<commit_message>
Implemented fuel saving techniques
</commit_message>
<xml_diff>
--- a/+Model/template.xlsx
+++ b/+Model/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LaptimeSimOCP\+Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452C3F20-E734-4B1B-B2E4-259268217AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2FA497-8B41-43FE-BC35-9D72680EB2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22944" yWindow="756" windowWidth="21660" windowHeight="11328" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{C9770ACA-89D6-4C25-A406-8CFD34B6BEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="MassInertia" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t>setup</t>
   </si>
@@ -176,15 +176,6 @@
   </si>
   <si>
     <t>maximum_torque</t>
-  </si>
-  <si>
-    <t>"-5% lltd"</t>
-  </si>
-  <si>
-    <t>"-15% lltd"</t>
-  </si>
-  <si>
-    <t>"-10% lltd"</t>
   </si>
 </sst>
 </file>
@@ -537,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E820AE81-6940-42C1-9794-755A660CF3D0}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,114 +607,6 @@
         <v>0.47</v>
       </c>
       <c r="K2">
-        <v>9.8059999999999992</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3">
-        <v>965</v>
-      </c>
-      <c r="D3">
-        <v>1400</v>
-      </c>
-      <c r="E3">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="F3">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="G3">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="H3">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="I3">
-        <v>0.316</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J5" si="0">0.47</f>
-        <v>0.47</v>
-      </c>
-      <c r="K3">
-        <v>9.8059999999999992</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4">
-        <v>965</v>
-      </c>
-      <c r="D4">
-        <v>1400</v>
-      </c>
-      <c r="E4">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="F4">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="G4">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="H4">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="I4">
-        <v>0.316</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="K4">
-        <v>9.8059999999999992</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5">
-        <v>965</v>
-      </c>
-      <c r="D5">
-        <v>1400</v>
-      </c>
-      <c r="E5">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="F5">
-        <v>3.7050000000000001</v>
-      </c>
-      <c r="G5">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="H5">
-        <v>4.4939999999999998</v>
-      </c>
-      <c r="I5">
-        <v>0.316</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="K5">
         <v>9.8059999999999992</v>
       </c>
     </row>
@@ -737,7 +620,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,13 +647,14 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3</v>
+        <f>1.1*2.9</f>
+        <v>3.19</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D2" t="s">
         <v>29</v>
@@ -778,13 +662,14 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <f t="shared" ref="A3:A5" si="0">1.1*2.9</f>
+        <v>3.19</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -792,13 +677,14 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>3.19</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -806,13 +692,14 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>3.19</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>450</v>
+        <v>550</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
@@ -1064,7 +951,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +978,7 @@
         <v>1.0029999999999999</v>
       </c>
       <c r="B2">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1.2250000000000001</v>
@@ -1354,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E935BBC8-6905-40C4-93AA-35113AE6796F}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,7 +1264,7 @@
         <v>0.7</v>
       </c>
       <c r="B2" s="1">
-        <v>5000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,7 +1273,7 @@
         <v>0.7</v>
       </c>
       <c r="B3" s="1">
-        <v>5001</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1395,7 +1282,7 @@
         <v>0.7</v>
       </c>
       <c r="B4" s="1">
-        <v>5002</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1291,7 @@
         <v>0.7</v>
       </c>
       <c r="B5" s="1">
-        <v>5003</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>